<commit_message>
Add Python debugger configuration, enhance OpenAI client initialization, and improve remediation list generator functionality
</commit_message>
<xml_diff>
--- a/philips_scorecard/io/philips_rules.xlsx
+++ b/philips_scorecard/io/philips_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sturner/Documents/Development/WITS/Applications/create_philips_scorecardOLD/philips_scorecard/io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sturner/Documents/Development/WITS/Functions/build_philips_scorecard/philips_scorecard/io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A5B253-0C58-D749-930C-07EE41C3A355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D3E7AE-0E04-4240-BC5E-FE894A138B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40460" yWindow="500" windowWidth="34340" windowHeight="25000" xr2:uid="{50391E7C-07C4-4370-8AE9-A55AEAB09019}"/>
+    <workbookView xWindow="42460" yWindow="500" windowWidth="34340" windowHeight="25000" xr2:uid="{50391E7C-07C4-4370-8AE9-A55AEAB09019}"/>
   </bookViews>
   <sheets>
     <sheet name="bp" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="235">
   <si>
     <t>Philips Requirements</t>
   </si>
@@ -1008,9 +1008,6 @@
   </si>
   <si>
     <t>Is WEP encryption in use on any SSIDs?</t>
-  </si>
-  <si>
-    <t>bp_5_2_justified</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1357,16 +1354,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1705,7 +1695,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2250,7 +2240,7 @@
         <v>72</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="37" t="s">
         <v>73</v>
@@ -2312,35 +2302,31 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="52" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A23" s="48">
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A23" s="35">
         <v>24</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="E23" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="G23" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="51" t="s">
+      <c r="E23" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="J23" s="51" t="s">
+      <c r="J23" s="37" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>